<commit_message>
This is a commit before class ending
</commit_message>
<xml_diff>
--- a/TestData/AutomationData.xlsx
+++ b/TestData/AutomationData.xlsx
@@ -9,15 +9,16 @@
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
-    <sheet name="Data3" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Emp" sheetId="4" r:id="rId4"/>
+    <sheet name="User" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Maven</t>
   </si>
@@ -50,6 +51,18 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Aswini101</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Hyd</t>
+  </si>
+  <si>
+    <t>Admin1</t>
   </si>
 </sst>
 </file>
@@ -494,14 +507,14 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -510,4 +523,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Update Dec 17
</commit_message>
<xml_diff>
--- a/TestData/AutomationData.xlsx
+++ b/TestData/AutomationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Maven</t>
   </si>
@@ -59,10 +59,28 @@
     <t>Selenium</t>
   </si>
   <si>
-    <t>Hyd</t>
-  </si>
-  <si>
-    <t>Admin1</t>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Capture.png</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>Aswini102</t>
+  </si>
+  <si>
+    <t>Aswini103</t>
+  </si>
+  <si>
+    <t>user2</t>
   </si>
 </sst>
 </file>
@@ -86,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,13 +127,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,15 +536,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -527,26 +557,108 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>101</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1">
+        <v>102</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Test for Search Emp List
</commit_message>
<xml_diff>
--- a/TestData/AutomationData.xlsx
+++ b/TestData/AutomationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Login" sheetId="3" r:id="rId3"/>
     <sheet name="Emp" sheetId="4" r:id="rId4"/>
     <sheet name="User" sheetId="5" r:id="rId5"/>
+    <sheet name="EmpList" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Maven</t>
   </si>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t>user2</t>
+  </si>
+  <si>
+    <t>Lisa</t>
   </si>
 </sst>
 </file>
@@ -559,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -676,4 +680,30 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Test Case for Apply Leave
</commit_message>
<xml_diff>
--- a/TestData/AutomationData.xlsx
+++ b/TestData/AutomationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Emp" sheetId="4" r:id="rId4"/>
     <sheet name="User" sheetId="5" r:id="rId5"/>
     <sheet name="EmpList" sheetId="6" r:id="rId6"/>
+    <sheet name="ApplyLeave" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Maven</t>
   </si>
@@ -85,6 +86,15 @@
   </si>
   <si>
     <t>Lisa</t>
+  </si>
+  <si>
+    <t>By.xpath("//*[text()='Leave Type ']//following::select[1]")</t>
+  </si>
+  <si>
+    <t>By.xpath("//table[contains(@class,'calendar')]//a[text()=25]")</t>
+  </si>
+  <si>
+    <t>I am out sick</t>
   </si>
 </sst>
 </file>
@@ -686,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,4 +716,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
@Mukesh-Please check my UpdateVacancy Test Case
</commit_message>
<xml_diff>
--- a/TestData/AutomationData.xlsx
+++ b/TestData/AutomationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="User" sheetId="5" r:id="rId5"/>
     <sheet name="EmpList" sheetId="6" r:id="rId6"/>
     <sheet name="ApplyLeave" sheetId="7" r:id="rId7"/>
+    <sheet name="Vacancy" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Maven</t>
   </si>
@@ -88,26 +89,29 @@
     <t>Lisa</t>
   </si>
   <si>
-    <t>By.xpath("//*[text()='Leave Type ']//following::select[1]")</t>
-  </si>
-  <si>
-    <t>By.xpath("//table[contains(@class,'calendar')]//a[text()=25]")</t>
-  </si>
-  <si>
     <t>I am out sick</t>
+  </si>
+  <si>
+    <t>US - Personal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,10 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,29 +725,53 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>